<commit_message>
multiple bools for an interval
</commit_message>
<xml_diff>
--- a/excel files/Escape_case_study.xlsx
+++ b/excel files/Escape_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDB4E3A-E2F1-4566-BA1D-375476200B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E133B9C9-601B-4282-9886-F95937093E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="740" yWindow="340" windowWidth="18090" windowHeight="8960" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="84">
   <si>
     <t>components</t>
   </si>
@@ -88,9 +88,6 @@
     <t xml:space="preserve">acetate </t>
   </si>
   <si>
-    <t xml:space="preserve">buytrate </t>
-  </si>
-  <si>
     <t>composition</t>
   </si>
   <si>
@@ -103,9 +100,6 @@
     <t>prop</t>
   </si>
   <si>
-    <t>ace, prop, but</t>
-  </si>
-  <si>
     <t>inputs</t>
   </si>
   <si>
@@ -121,9 +115,6 @@
     <t>propionate</t>
   </si>
   <si>
-    <t>buytrate</t>
-  </si>
-  <si>
     <t>ace,prop</t>
   </si>
   <si>
@@ -133,9 +124,6 @@
     <t>seperation_coef</t>
   </si>
   <si>
-    <t>[1,0,0]; [0,1,0]; [0,0,1]</t>
-  </si>
-  <si>
     <t>[1,0];[0,1]</t>
   </si>
   <si>
@@ -145,18 +133,12 @@
     <t>sep2</t>
   </si>
   <si>
-    <t>sep3</t>
-  </si>
-  <si>
     <t>P_pro_batch</t>
   </si>
   <si>
     <t>energy</t>
   </si>
   <si>
-    <t>carbon_input</t>
-  </si>
-  <si>
     <t>casine</t>
   </si>
   <si>
@@ -166,9 +148,6 @@
     <t>input_bounds</t>
   </si>
   <si>
-    <t>{'pH':[5,8]}</t>
-  </si>
-  <si>
     <t xml:space="preserve">layer </t>
   </si>
   <si>
@@ -217,9 +196,6 @@
     <t>output_abrr</t>
   </si>
   <si>
-    <t>Ex_S_cpd00027_ext</t>
-  </si>
-  <si>
     <t>abbreviation</t>
   </si>
   <si>
@@ -259,18 +235,12 @@
     <t>Ex_S_cpd00141_ext, Ex_S_cpd00029_ext</t>
   </si>
   <si>
-    <t>D-Glucose</t>
-  </si>
-  <si>
     <t>Propionate, Acetate</t>
   </si>
   <si>
     <t>open_fermentation</t>
   </si>
   <si>
-    <t>Glucose_open_fermentation.json</t>
-  </si>
-  <si>
     <t>Propionate, Acetate, Butyrate</t>
   </si>
   <si>
@@ -289,10 +259,37 @@
     <t>is_SBML (not really used)</t>
   </si>
   <si>
-    <t>carbon_fructose</t>
-  </si>
-  <si>
-    <t>inputBool</t>
+    <t>yield_of</t>
+  </si>
+  <si>
+    <t>fru</t>
+  </si>
+  <si>
+    <t>open_fermentation_polynomial_ESCAPE33.json</t>
+  </si>
+  <si>
+    <t>ace, prop</t>
+  </si>
+  <si>
+    <t>fructose</t>
+  </si>
+  <si>
+    <t>carbon_input1</t>
+  </si>
+  <si>
+    <t>carbon_input2</t>
+  </si>
+  <si>
+    <t>{'pH':[5,8.5]}</t>
+  </si>
+  <si>
+    <t>Ex_S_cpd00027_ext, Ex_S_cpd00082_ext</t>
+  </si>
+  <si>
+    <t>D-Glucose, D-Fructose</t>
+  </si>
+  <si>
+    <t>glu,fru</t>
   </si>
 </sst>
 </file>
@@ -329,7 +326,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,12 +336,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -407,26 +398,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -435,8 +425,12 @@
     </xf>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,15 +909,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>527050</xdr:colOff>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>143510</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>16510</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -938,8 +932,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="527050" y="1600200"/>
-          <a:ext cx="4442460" cy="3543300"/>
+          <a:off x="400050" y="1593850"/>
+          <a:ext cx="5204460" cy="3543300"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1071,6 +1065,113 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>146050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>226060</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CuadroTexto 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D69AA09C-48BE-4E02-8F90-661FCE1F8C2B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5772150" y="1619250"/>
+          <a:ext cx="5204460" cy="1333500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>YIELD</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> OF </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>the sum of what the conversion factor or yield needs to be multiplied by</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>one component:                   glu </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>multiple components: (glu + prot)  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>CAREFULL don't forget brackets whith multiple components </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1078,15 +1179,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>414655</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>32383</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>138430</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>73660</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1220,7 +1321,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1516,13 +1617,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -1560,15 +1661,15 @@
         <v>0</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="9">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
-        <v>38</v>
+      <c r="B2" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -1582,90 +1683,94 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>18</v>
+      <c r="G2" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="10">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3">
+        <v>100</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+      <c r="E3">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="10">
+      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
+      <c r="B5" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="10">
-        <v>3</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>24</v>
+      <c r="G5" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
+    </row>
+    <row r="6" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="17"/>
+      <c r="G6" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1685,18 +1790,18 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.6328125" customWidth="1"/>
     <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="7" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.90625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.90625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.1796875" customWidth="1"/>
@@ -1710,28 +1815,28 @@
         <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -1743,252 +1848,252 @@
         <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="5">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="6">
-        <v>0</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="C2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="6">
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="5">
+        <v>100</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="5">
         <v>1</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="6" t="s">
+      <c r="H3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5">
+        <v>100</v>
+      </c>
+      <c r="L3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="6">
-        <v>0</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="M3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
         <v>100</v>
       </c>
-      <c r="L2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="6">
+      <c r="L4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="6">
+    <row r="5" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="C5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="6">
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
+        <v>100</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="5">
         <v>1</v>
       </c>
-      <c r="H3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="6" t="s">
+      <c r="H6" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="5">
+        <v>100</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
+      <c r="M6" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="5">
         <v>100</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="6">
-        <v>2</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="L7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>100</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M4" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="6">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>100</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M5" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>100</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B7" s="6">
-        <v>2</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
-        <v>100</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="6">
+      <c r="M7" s="5">
         <v>2</v>
       </c>
     </row>
@@ -2006,181 +2111,203 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8D8FB7-0FD2-42C3-9D82-0A6D9AE32488}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
+    <col min="6" max="6" width="35.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G2" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="14">
+        <v>0</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="D7" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="15">
-        <v>0</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="E7" s="16">
-        <v>0</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>78</v>
+      <c r="E7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -2191,16 +2318,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9730D4B9-BF36-445D-9853-EF3DA446843F}">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
@@ -2209,18 +2336,18 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="13" max="13" width="8.81640625" customWidth="1"/>
+    <col min="12" max="12" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -2235,48 +2362,45 @@
         <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>51</v>
+      <c r="E2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -2284,37 +2408,34 @@
       <c r="K2" s="1">
         <v>0</v>
       </c>
-      <c r="L2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>51</v>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>44</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -2322,11 +2443,8 @@
       <c r="K3" s="1">
         <v>0</v>
       </c>
-      <c r="L3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2354,17 +2472,14 @@
       <c r="I4" s="1">
         <v>0</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2392,17 +2507,14 @@
       <c r="I5" s="1">
         <v>0</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2430,17 +2542,14 @@
       <c r="I6" s="3">
         <v>0</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2468,19 +2577,16 @@
       <c r="I7" s="1">
         <v>0</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -2506,19 +2612,16 @@
       <c r="I8" s="1">
         <v>0</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -2544,19 +2647,16 @@
       <c r="I9" s="1">
         <v>0</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="J9" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1">
         <v>0</v>
@@ -2588,13 +2688,10 @@
       <c r="K10" s="1">
         <v>0</v>
       </c>
-      <c r="L10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
@@ -2624,53 +2721,12 @@
         <v>0</v>
       </c>
       <c r="K11" s="1">
-        <v>0</v>
-      </c>
-      <c r="L11" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="1">
-        <v>0</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1">
-        <v>0</v>
-      </c>
-      <c r="E12" s="1">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0</v>
-      </c>
-      <c r="I12" s="1">
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1">
-        <v>0</v>
-      </c>
-      <c r="L12" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="B13:H15 I15">
+  <conditionalFormatting sqref="B12:H14 I14">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -2680,7 +2736,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13:J14">
+  <conditionalFormatting sqref="J12:J13">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -2690,8 +2746,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:M12">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="B2:L11">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2708,41 +2764,41 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFEA29F-1D3A-4383-97E1-D31836BA3887}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>61</v>
+      <c r="A1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -2750,7 +2806,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -2758,26 +2814,34 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
-        <v>68</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reorganising + multiple bools per interval
</commit_message>
<xml_diff>
--- a/excel files/Escape_case_study.xlsx
+++ b/excel files/Escape_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E133B9C9-601B-4282-9886-F95937093E05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74607162-705E-49D2-8D21-5E50CF40D4B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="340" windowWidth="18090" windowHeight="8960" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="683" activeTab="4" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="85">
   <si>
     <t>components</t>
   </si>
@@ -160,15 +160,6 @@
     <t>[0,1000]</t>
   </si>
   <si>
-    <t>P_sherm_model.xml</t>
-  </si>
-  <si>
-    <t>PAC_4875_model.xml</t>
-  </si>
-  <si>
-    <t>P_acnes_model.xml</t>
-  </si>
-  <si>
     <t>utility_price</t>
   </si>
   <si>
@@ -226,12 +217,6 @@
     <t>prop, ace</t>
   </si>
   <si>
-    <t>P_avidum_model.xml</t>
-  </si>
-  <si>
-    <t>P_propionicum_model.xml</t>
-  </si>
-  <si>
     <t>Ex_S_cpd00141_ext, Ex_S_cpd00029_ext</t>
   </si>
   <si>
@@ -290,6 +275,24 @@
   </si>
   <si>
     <t>glu,fru</t>
+  </si>
+  <si>
+    <t>glu, fru</t>
+  </si>
+  <si>
+    <t>PAC_4875_model.json</t>
+  </si>
+  <si>
+    <t>P_sherm_model.json</t>
+  </si>
+  <si>
+    <t>P_avidum_model.json</t>
+  </si>
+  <si>
+    <t>P_acnes_model.json</t>
+  </si>
+  <si>
+    <t>P_propionicum_model.json</t>
   </si>
 </sst>
 </file>
@@ -398,7 +401,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -429,6 +432,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1620,7 +1626,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1669,16 +1675,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C2">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>100</v>
       </c>
       <c r="E2">
-        <v>1.0000000000000001E-5</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1695,22 +1701,22 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C3">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <v>100</v>
       </c>
       <c r="E3">
-        <v>1.0000000000000001E-5</v>
+        <v>0.39</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1733,7 +1739,7 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1.0000000000000001E-5</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>21</v>
@@ -1759,7 +1765,7 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>1.26</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>19</v>
@@ -1790,7 +1796,7 @@
   <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1802,7 +1808,7 @@
     <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.1796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.1796875" customWidth="1"/>
     <col min="11" max="11" width="17.1796875" bestFit="1" customWidth="1"/>
@@ -1830,7 +1836,7 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>38</v>
@@ -1848,7 +1854,7 @@
         <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
@@ -1862,7 +1868,7 @@
         <v>39</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="E2" s="5">
         <v>0</v>
@@ -1874,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>28</v>
@@ -1903,7 +1909,7 @@
         <v>39</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -1915,7 +1921,7 @@
         <v>1</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>28</v>
@@ -1944,7 +1950,7 @@
         <v>39</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -1956,7 +1962,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>28</v>
@@ -1985,7 +1991,7 @@
         <v>39</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -1997,7 +2003,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>28</v>
@@ -2026,7 +2032,7 @@
         <v>39</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>17</v>
+        <v>79</v>
       </c>
       <c r="E6" s="5">
         <v>0</v>
@@ -2038,7 +2044,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>28</v>
@@ -2058,7 +2064,7 @@
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
@@ -2067,19 +2073,19 @@
         <v>39</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="G7" s="5">
         <v>0</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>28</v>
@@ -2114,12 +2120,12 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.36328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.90625" customWidth="1"/>
@@ -2130,172 +2136,172 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>48</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
-        <v>41</v>
+        <v>80</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
-        <v>40</v>
+        <v>81</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
-        <v>42</v>
+        <v>83</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B7" s="14">
         <v>0</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>17</v>
@@ -2304,10 +2310,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2320,8 +2326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9730D4B9-BF36-445D-9853-EF3DA446843F}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2344,10 +2350,10 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D1" t="s">
         <v>11</v>
@@ -2365,7 +2371,7 @@
         <v>31</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
         <v>23</v>
@@ -2376,7 +2382,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
@@ -2400,7 +2406,7 @@
         <v>26</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -2411,7 +2417,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -2434,8 +2440,8 @@
       <c r="H3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="6" t="s">
-        <v>44</v>
+      <c r="I3" s="18">
+        <v>0</v>
       </c>
       <c r="J3" s="1">
         <v>0</v>
@@ -2621,7 +2627,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1">
         <v>0</v>
@@ -2766,18 +2772,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BFEA29F-1D3A-4383-97E1-D31836BA3887}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -2785,15 +2791,15 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
         <v>55</v>
-      </c>
-      <c r="B3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -2806,7 +2812,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -2817,7 +2823,7 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
@@ -2825,23 +2831,23 @@
         <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
surrogate models case study
</commit_message>
<xml_diff>
--- a/excel files/Escape_case_study.xlsx
+++ b/excel files/Escape_case_study.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751DC152-4BE4-4ECE-A72D-C6E32CE89ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E3D126-4B3E-4918-A44F-25A0217A2BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4970" yWindow="450" windowWidth="12570" windowHeight="6230" tabRatio="683" activeTab="2" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
-    <sheet name="reactor_intervals" sheetId="2" r:id="rId2"/>
+    <sheet name="process_intervals" sheetId="2" r:id="rId2"/>
     <sheet name="models" sheetId="14" r:id="rId3"/>
     <sheet name="connection_matrix" sheetId="11" r:id="rId4"/>
     <sheet name="abbr" sheetId="15" r:id="rId5"/>
@@ -1633,6 +1633,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>219185</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>176389</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>598252</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>144794</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24F44E08-9D8D-5EB7-4127-729A84FCB11F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5045185" y="2194278"/>
+          <a:ext cx="5240345" cy="2720072"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2331,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2DC50F-7E38-4E45-9660-C41E1DA6142A}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2655,7 +2699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F8D8FB7-0FD2-42C3-9D82-0A6D9AE32488}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -2863,7 +2907,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
adding separation processes as stand-alone intervals
</commit_message>
<xml_diff>
--- a/excel files/Escape_case_study.xlsx
+++ b/excel files/Escape_case_study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83E3D126-4B3E-4918-A44F-25A0217A2BB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F93E5A7-3D82-468C-AC68-6E45F07FBCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="3" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="input_output_intervals" sheetId="1" r:id="rId1"/>
@@ -2375,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2DC50F-7E38-4E45-9660-C41E1DA6142A}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2906,7 +2906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9730D4B9-BF36-445D-9853-EF3DA446843F}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>